<commit_message>
Sprint 5 - 2
</commit_message>
<xml_diff>
--- a/Spring_4/FO.RT.GDC.SDC.004-001.xlsx
+++ b/Spring_4/FO.RT.GDC.SDC.004-001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sdc-docs\Spring_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sdc-docs\Spring_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -249,6 +249,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -266,30 +290,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,7 +574,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A1:E28"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,23 +587,23 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10">
-        <v>43362</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="18">
+        <v>43392</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -612,218 +612,218 @@
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="A29:E29"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B9:E9"/>
@@ -838,11 +838,11 @@
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A19:E19"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="A28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>